<commit_message>
Version 1.0 after prototype soldering
</commit_message>
<xml_diff>
--- a/hardware/documentation/BOM Hittestress Homerus 2023.xlsx
+++ b/hardware/documentation/BOM Hittestress Homerus 2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drasv\github\aid-hittestress-2023\hardware\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{362BAA85-F8DA-4CC1-9871-EC0540510661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D68A638-F43C-4612-8A8C-A1ABD5327348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29715" yWindow="915" windowWidth="18900" windowHeight="10980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -338,213 +338,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>745620</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>162930</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>916560</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>168435</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="face-happy">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="4288920" y="2877555"/>
-          <a:ext cx="170940" cy="186480"/>
-          <a:chOff x="4373280" y="2788200"/>
-          <a:chExt cx="178560" cy="178560"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="Ovaal 2">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="4373280" y="2788200"/>
-            <a:ext cx="178560" cy="178560"/>
-          </a:xfrm>
-          <a:prstGeom prst="ellipse">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="77BC65">
-              <a:alpha val="50000"/>
-            </a:srgbClr>
-          </a:solidFill>
-          <a:ln w="6480">
-            <a:solidFill>
-              <a:srgbClr val="069A2E"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor"/>
-        </xdr:style>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="4" name="Ovaal 3">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="4484160" y="2841120"/>
-            <a:ext cx="23040" cy="23040"/>
-          </a:xfrm>
-          <a:prstGeom prst="ellipse">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="6480">
-            <a:solidFill>
-              <a:srgbClr val="069A2E"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor"/>
-        </xdr:style>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="Ovaal 4">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="4417920" y="2841480"/>
-            <a:ext cx="23400" cy="23040"/>
-          </a:xfrm>
-          <a:prstGeom prst="ellipse">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="6480">
-            <a:solidFill>
-              <a:srgbClr val="069A2E"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor"/>
-        </xdr:style>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="Boog 5">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm rot="10800000">
-            <a:off x="4408920" y="2856960"/>
-            <a:ext cx="110160" cy="69840"/>
-          </a:xfrm>
-          <a:prstGeom prst="arc">
-            <a:avLst>
-              <a:gd name="adj1" fmla="val 10432394"/>
-              <a:gd name="adj2" fmla="val 295364"/>
-            </a:avLst>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="6480">
-            <a:solidFill>
-              <a:srgbClr val="069A2E"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor"/>
-        </xdr:style>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -847,7 +640,7 @@
   <dimension ref="B2:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1153,6 +946,5 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>